<commit_message>
Few changes here and there
</commit_message>
<xml_diff>
--- a/Solitaire/Assignment/graph.xlsx
+++ b/Solitaire/Assignment/graph.xlsx
@@ -183,6 +183,12 @@
                 <c:pt idx="9">
                   <c:v>40</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -221,6 +227,12 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>823162</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14987773</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>114544918</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -235,8 +247,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="166728832"/>
-        <c:axId val="166730752"/>
+        <c:axId val="196924928"/>
+        <c:axId val="196926848"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -283,6 +295,12 @@
                 <c:pt idx="9">
                   <c:v>40</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -321,6 +339,12 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>986</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11446</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>101556</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -335,11 +359,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="166747136"/>
-        <c:axId val="166745216"/>
+        <c:axId val="197070208"/>
+        <c:axId val="197068288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="166728832"/>
+        <c:axId val="196924928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -368,12 +392,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166730752"/>
+        <c:crossAx val="196926848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="166730752"/>
+        <c:axId val="196926848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -403,12 +427,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166728832"/>
+        <c:crossAx val="196924928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="166745216"/>
+        <c:axId val="197068288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -437,12 +461,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166747136"/>
+        <c:crossAx val="197070208"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="166747136"/>
+        <c:axId val="197070208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -452,7 +476,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166745216"/>
+        <c:crossAx val="197068288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -799,7 +823,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,7 +1065,27 @@
         <v>6</v>
       </c>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>44</v>
+      </c>
+      <c r="E12">
+        <v>14987773</v>
+      </c>
+      <c r="F12">
+        <v>11446</v>
+      </c>
+    </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>48</v>
+      </c>
+      <c r="E13">
+        <v>114544918</v>
+      </c>
+      <c r="F13">
+        <v>101556</v>
+      </c>
       <c r="G13">
         <v>6</v>
       </c>

</xml_diff>